<commit_message>
Add generic file to config
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hettnekm1/OAscript/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C661674A-C7A9-3A4B-81B5-B82FF4C57A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0108A0E-9F7B-EE4A-AD68-55372D35CFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>File 1</t>
   </si>
@@ -39,13 +39,37 @@
     <t>File 2</t>
   </si>
   <si>
-    <t>Name of file</t>
-  </si>
-  <si>
-    <t>2018_Monitoring_OA___basislijst_2-aangepast_20190311.xls</t>
-  </si>
-  <si>
     <t>filename</t>
+  </si>
+  <si>
+    <t>ID column</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ISSN</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>ID-1</t>
+  </si>
+  <si>
+    <t>Title of the contribution in original language-2</t>
+  </si>
+  <si>
+    <t>Journal &gt; ISSN-5</t>
+  </si>
+  <si>
+    <t>Electronic version(s) of this work &gt; DOI (Digital Object Identifier)-6</t>
+  </si>
+  <si>
+    <t>scopus_social_evol_2018.csv</t>
   </si>
 </sst>
 </file>
@@ -397,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD2166A-EC47-ED44-87CF-C15299393BC9}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -419,13 +443,45 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>